<commit_message>
Add test models and code snippets
</commit_message>
<xml_diff>
--- a/core/esmf-aspect-meta-model-python/esmf_aspect_meta_model_python/pydentic/aspect_model_examples.xlsx
+++ b/core/esmf-aspect-meta-model-python/esmf_aspect_meta_model_python/pydentic/aspect_model_examples.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\BoschSDK\git\bci-oss\esmf-sdk-py-aspect-model-loader\core\esmf-aspect-meta-model-python\esmf_aspect_meta_model_python\pydentic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8B6D9C0-D7D1-4363-9979-D071DAF2F899}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8DEC23D-422A-45AD-8D6B-71B0ACAB3055}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="test models" sheetId="2" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'test models'!$A$1:$B$1</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,72 +28,138 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
-  <si>
-    <t>Node</t>
-  </si>
-  <si>
-    <t>Characteristics</t>
-  </si>
-  <si>
-    <t>Test model file</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="44">
   <si>
     <t>Collection</t>
   </si>
   <si>
-    <t>list</t>
-  </si>
-  <si>
-    <t>set</t>
-  </si>
-  <si>
-    <t>sorted set</t>
-  </si>
-  <si>
-    <t>Class name</t>
-  </si>
-  <si>
-    <t>Parent class name</t>
-  </si>
-  <si>
-    <t>Note</t>
-  </si>
-  <si>
-    <t>time series</t>
-  </si>
-  <si>
-    <t>List</t>
-  </si>
-  <si>
-    <t>Set</t>
-  </si>
-  <si>
-    <t>duplicate elements</t>
-  </si>
-  <si>
-    <t>ordered</t>
-  </si>
-  <si>
-    <t>SAMM</t>
-  </si>
-  <si>
-    <t>urn:samm:org.eclipse.esmf.samm:characteristic:2.1.0#List</t>
-  </si>
-  <si>
-    <t>urn:samm:org.eclipse.esmf.samm:characteristic:2.1.0#Set</t>
-  </si>
-  <si>
-    <t>urn:samm:org.eclipse.esmf.samm:characteristic:2.1.0#SortedSet</t>
-  </si>
-  <si>
     <t>SortedSet</t>
   </si>
   <si>
-    <t>TimeSeries</t>
-  </si>
-  <si>
-    <t>containing values with the exact point in time when the values where recorded</t>
+    <t>file name</t>
+  </si>
+  <si>
+    <t>test model</t>
+  </si>
+  <si>
+    <t>aspect.py</t>
+  </si>
+  <si>
+    <t>Aspect.ttl</t>
+  </si>
+  <si>
+    <t>SAMM type to check</t>
+  </si>
+  <si>
+    <t>Aspect</t>
+  </si>
+  <si>
+    <t>AspectWithCollection.ttl</t>
+  </si>
+  <si>
+    <t>aspect_with_collection.py</t>
+  </si>
+  <si>
+    <t>AspectWithCollections.ttl</t>
+  </si>
+  <si>
+    <t>aspect_with_collections.py</t>
+  </si>
+  <si>
+    <t>aspect_with_optional_property.py</t>
+  </si>
+  <si>
+    <t>AspectWithOptionalProperty.ttl</t>
+  </si>
+  <si>
+    <t>Property</t>
+  </si>
+  <si>
+    <t>optional</t>
+  </si>
+  <si>
+    <t>Set, List</t>
+  </si>
+  <si>
+    <t>AspectWithOptionalProperties.ttl</t>
+  </si>
+  <si>
+    <t>aspect_with_optional_properties.py</t>
+  </si>
+  <si>
+    <t>Properties</t>
+  </si>
+  <si>
+    <t>aspect_with_enumeration.py</t>
+  </si>
+  <si>
+    <t>AspectWithEnumeration.ttl</t>
+  </si>
+  <si>
+    <t>Enumeration</t>
+  </si>
+  <si>
+    <t>aspect_with_constraint.py</t>
+  </si>
+  <si>
+    <t>aspect_with_encoding_constraint.py</t>
+  </si>
+  <si>
+    <t>aspect_with_fixed_point_constraint.py</t>
+  </si>
+  <si>
+    <t>aspect_with_language_constraint.py</t>
+  </si>
+  <si>
+    <t>AspectWithConstraint.ttl</t>
+  </si>
+  <si>
+    <t>LengthConstraint, RangeConstraint, RegularExpressionConstraint</t>
+  </si>
+  <si>
+    <t>AspectWithEncodingConstraint.ttl</t>
+  </si>
+  <si>
+    <t>EncodingConstraint</t>
+  </si>
+  <si>
+    <t>AspectWithFixedPointConstraint.ttl</t>
+  </si>
+  <si>
+    <t>FixedPointConstraint</t>
+  </si>
+  <si>
+    <t>Constraint</t>
+  </si>
+  <si>
+    <t>AspectWithLanguageConstraint.ttl</t>
+  </si>
+  <si>
+    <t>LanguageConstraint</t>
+  </si>
+  <si>
+    <t>aspect_with_sorted_set.py</t>
+  </si>
+  <si>
+    <t>aspect_with_time_series.py</t>
+  </si>
+  <si>
+    <t>AspectWithSortedSet.ttl</t>
+  </si>
+  <si>
+    <t>AspectWithTimeSeries.ttl</t>
+  </si>
+  <si>
+    <t>TimeSeriesEntity</t>
+  </si>
+  <si>
+    <t>aspect_with_entity.py</t>
+  </si>
+  <si>
+    <t>AspectWithEntity.ttl</t>
+  </si>
+  <si>
+    <t>SingleEntity, Entity</t>
   </si>
 </sst>
 </file>
@@ -134,17 +203,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,152 +485,205 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32D1B94C-1B98-40CD-9D94-971C627A4A5C}">
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="4" t="s">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="2" t="s">
+      <c r="D5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E3" t="b">
-        <v>1</v>
-      </c>
-      <c r="H3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H4" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="C8" t="s">
         <v>19</v>
       </c>
-      <c r="C5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E5" t="b">
-        <v>1</v>
-      </c>
-      <c r="H5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>20</v>
       </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="B9" t="s">
         <v>21</v>
       </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" t="s">
+        <v>43</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
-  </mergeCells>
+  <autoFilter ref="A1:B1" xr:uid="{32D1B94C-1B98-40CD-9D94-971C627A4A5C}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>